<commit_message>
Add RADAR4Chem and Chemotion Repository
</commit_message>
<xml_diff>
--- a/graph/legacy/Repositories.xlsx
+++ b/graph/legacy/Repositories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p.ost/Documents/Projekte/DCE-NG/graph/legacy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3012FB21-0DE2-614D-B276-7887B28ABE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E94567E-D100-8740-BA52-33BB02256BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10340" yWindow="8560" windowWidth="36280" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="364">
   <si>
     <t>Hosting Institution</t>
   </si>
@@ -1092,6 +1092,27 @@
   </si>
   <si>
     <t>Publication and (long term) archiving of research data from participating institutions in Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Chemotion Repository</t>
+  </si>
+  <si>
+    <t>https://www.chemotion-repository.net</t>
+  </si>
+  <si>
+    <t>Chemotion Repository provides an archive for materials, as well as research data repository for samples, reactions and analyses</t>
+  </si>
+  <si>
+    <t>FIZ Karlsruhe</t>
+  </si>
+  <si>
+    <t>RADAR4Chem</t>
+  </si>
+  <si>
+    <t>https://radar4chem.radar-service.eu</t>
+  </si>
+  <si>
+    <t>API access only includes metadata</t>
   </si>
 </sst>
 </file>
@@ -1932,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3258,16 +3279,16 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>353</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>357</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E54" t="s">
         <v>26</v>
@@ -3276,21 +3297,24 @@
         <v>26</v>
       </c>
       <c r="I54" t="s">
-        <v>179</v>
+        <v>358</v>
+      </c>
+      <c r="J54" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>360</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>361</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E55" t="s">
         <v>26</v>
@@ -3299,61 +3323,64 @@
         <v>26</v>
       </c>
       <c r="I55" t="s">
-        <v>181</v>
+        <v>362</v>
+      </c>
+      <c r="J55" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>347</v>
+        <v>178</v>
       </c>
       <c r="E56" t="s">
         <v>26</v>
       </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
       <c r="I56" t="s">
-        <v>183</v>
-      </c>
-      <c r="J56" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>348</v>
+        <v>178</v>
       </c>
       <c r="E57" t="s">
         <v>26</v>
       </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
       <c r="I57" t="s">
-        <v>183</v>
-      </c>
-      <c r="J57" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>334</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -3364,25 +3391,19 @@
       <c r="E58" t="s">
         <v>26</v>
       </c>
-      <c r="F58" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" t="s">
-        <v>346</v>
-      </c>
       <c r="I58" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J58" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>334</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -3393,22 +3414,16 @@
       <c r="E59" t="s">
         <v>26</v>
       </c>
-      <c r="F59" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" t="s">
-        <v>346</v>
-      </c>
       <c r="I59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J59" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B60" t="s">
         <v>185</v>
@@ -3437,7 +3452,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B61" t="s">
         <v>185</v>
@@ -3466,16 +3481,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="B62" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="D62" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="E62" t="s">
         <v>26</v>
@@ -3483,94 +3498,103 @@
       <c r="F62" t="s">
         <v>26</v>
       </c>
+      <c r="G62" t="s">
+        <v>346</v>
+      </c>
       <c r="I62" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J62" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C63" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>348</v>
       </c>
       <c r="E63" t="s">
         <v>26</v>
       </c>
+      <c r="F63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" t="s">
+        <v>346</v>
+      </c>
       <c r="I63" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="J63" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B64" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E64" t="s">
         <v>26</v>
       </c>
+      <c r="F64" t="s">
+        <v>26</v>
+      </c>
       <c r="I64" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="J64" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>324</v>
+        <v>188</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="D65" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E65" t="s">
         <v>26</v>
       </c>
-      <c r="G65" t="s">
-        <v>29</v>
-      </c>
       <c r="I65" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="J65" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="D66" t="s">
         <v>199</v>
@@ -3578,250 +3602,238 @@
       <c r="E66" t="s">
         <v>26</v>
       </c>
-      <c r="G66" t="s">
-        <v>29</v>
-      </c>
       <c r="I66" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J66" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>210</v>
+        <v>324</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>212</v>
+        <v>25</v>
       </c>
       <c r="D67" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
         <v>26</v>
       </c>
+      <c r="G67" t="s">
+        <v>29</v>
+      </c>
       <c r="I67" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J67" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B68" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="E68" t="s">
         <v>26</v>
       </c>
-      <c r="F68" t="s">
-        <v>26</v>
+      <c r="G68" t="s">
+        <v>29</v>
       </c>
       <c r="I68" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="J68" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>326</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="D69" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="E69" t="s">
         <v>26</v>
       </c>
-      <c r="F69" t="s">
-        <v>26</v>
-      </c>
       <c r="I69" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J69" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="E70" t="s">
         <v>26</v>
       </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
       <c r="I70" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="J70" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>326</v>
       </c>
       <c r="B71" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>228</v>
+        <v>75</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
       </c>
       <c r="F71" t="s">
         <v>26</v>
       </c>
       <c r="I71" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="J71" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="B72" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E72" t="s">
         <v>26</v>
       </c>
       <c r="I72" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J72" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>336</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C73" t="s">
-        <v>165</v>
+        <v>22</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
-      </c>
-      <c r="E73" t="s">
+        <v>228</v>
+      </c>
+      <c r="F73" t="s">
         <v>26</v>
       </c>
       <c r="I73" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J73" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>234</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C74" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
         <v>26</v>
       </c>
-      <c r="F74" t="s">
-        <v>26</v>
-      </c>
-      <c r="G74" t="s">
-        <v>236</v>
-      </c>
-      <c r="H74">
-        <v>300</v>
-      </c>
       <c r="I74" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="J74" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>336</v>
       </c>
       <c r="B75" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E75" t="s">
         <v>26</v>
       </c>
-      <c r="F75" t="s">
-        <v>26</v>
-      </c>
-      <c r="G75" t="s">
-        <v>29</v>
-      </c>
-      <c r="H75">
-        <v>20</v>
-      </c>
       <c r="I75" t="s">
-        <v>241</v>
+        <v>232</v>
+      </c>
+      <c r="J75" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="B76" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C76" t="s">
         <v>25</v>
@@ -3836,24 +3848,27 @@
         <v>26</v>
       </c>
       <c r="G76" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H76">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="I76" t="s">
-        <v>244</v>
+        <v>237</v>
+      </c>
+      <c r="J76" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C77" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -3861,25 +3876,28 @@
       <c r="E77" t="s">
         <v>26</v>
       </c>
+      <c r="F77" t="s">
+        <v>26</v>
+      </c>
       <c r="G77" t="s">
         <v>29</v>
       </c>
+      <c r="H77">
+        <v>20</v>
+      </c>
       <c r="I77" t="s">
-        <v>247</v>
-      </c>
-      <c r="J77" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>245</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C78" t="s">
-        <v>341</v>
+        <v>25</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
@@ -3887,14 +3905,17 @@
       <c r="E78" t="s">
         <v>26</v>
       </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
       <c r="G78" t="s">
-        <v>29</v>
+        <v>243</v>
+      </c>
+      <c r="H78">
+        <v>50</v>
       </c>
       <c r="I78" t="s">
-        <v>247</v>
-      </c>
-      <c r="J78" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -3902,10 +3923,10 @@
         <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C79" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -3916,25 +3937,22 @@
       <c r="G79" t="s">
         <v>29</v>
       </c>
-      <c r="H79">
-        <v>2</v>
-      </c>
       <c r="I79" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="J79" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C80" t="s">
-        <v>25</v>
+        <v>341</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
@@ -3942,94 +3960,149 @@
       <c r="E80" t="s">
         <v>26</v>
       </c>
-      <c r="F80" t="s">
-        <v>26</v>
-      </c>
-      <c r="H80" t="s">
-        <v>254</v>
+      <c r="G80" t="s">
+        <v>29</v>
       </c>
       <c r="I80" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J80" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="G81" t="s">
+        <v>29</v>
+      </c>
+      <c r="H81">
+        <v>2</v>
       </c>
       <c r="I81" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="J81" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C82" t="s">
-        <v>341</v>
+        <v>25</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F82" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="H82" t="s">
+        <v>254</v>
       </c>
       <c r="I82" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J82" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>315</v>
+        <v>257</v>
       </c>
       <c r="B83" t="s">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F83" t="s">
         <v>155</v>
       </c>
       <c r="I83" t="s">
+        <v>259</v>
+      </c>
+      <c r="J83" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>257</v>
+      </c>
+      <c r="B84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C84" t="s">
+        <v>341</v>
+      </c>
+      <c r="D84" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" t="s">
+        <v>155</v>
+      </c>
+      <c r="I84" t="s">
+        <v>259</v>
+      </c>
+      <c r="J84" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>315</v>
+      </c>
+      <c r="B85" t="s">
+        <v>316</v>
+      </c>
+      <c r="C85" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" t="s">
+        <v>155</v>
+      </c>
+      <c r="I85" t="s">
         <v>317</v>
       </c>
-      <c r="J83" t="s">
+      <c r="J85" t="s">
         <v>318</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Repositories.xslx to reflect recent updates
</commit_message>
<xml_diff>
--- a/graph/legacy/Repositories.xlsx
+++ b/graph/legacy/Repositories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p.ost/Documents/Projekte/DCE-NG/graph/legacy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E94567E-D100-8740-BA52-33BB02256BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CABCB1-B1AD-F844-8610-E92DF567F2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="8560" windowWidth="36280" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repositories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="370">
   <si>
     <t>Hosting Institution</t>
   </si>
@@ -1113,6 +1113,24 @@
   </si>
   <si>
     <t>API access only includes metadata</t>
+  </si>
+  <si>
+    <t>NFDI-MatWerk Repository</t>
+  </si>
+  <si>
+    <t>https://matwerk.datamanager.kit.edu</t>
+  </si>
+  <si>
+    <t>Data and metadata repository for NFDI-MatWerk. File size limit for the metadata repository is 10MB.</t>
+  </si>
+  <si>
+    <t>Inorganic Crystal Structure Database</t>
+  </si>
+  <si>
+    <t>https://icsd.products.fiz-karlsruhe.de</t>
+  </si>
+  <si>
+    <t>Database for completely identified inorganic crystal structures. Access requires a license.</t>
   </si>
 </sst>
 </file>
@@ -1953,10 +1971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3175,16 +3193,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>353</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="C50" t="s">
         <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
@@ -3192,48 +3210,51 @@
       <c r="F50" t="s">
         <v>26</v>
       </c>
+      <c r="G50" t="s">
+        <v>29</v>
+      </c>
       <c r="I50" t="s">
-        <v>161</v>
+        <v>365</v>
       </c>
       <c r="J50" t="s">
-        <v>162</v>
+        <v>366</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>360</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>367</v>
       </c>
       <c r="C51" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" t="s">
-        <v>29</v>
+        <v>155</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
       </c>
       <c r="I51" t="s">
-        <v>166</v>
+        <v>368</v>
       </c>
       <c r="J51" t="s">
-        <v>167</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="D52" t="s">
         <v>160</v>
@@ -3241,22 +3262,25 @@
       <c r="E52" t="s">
         <v>26</v>
       </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
       <c r="I52" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="J52" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
         <v>160</v>
@@ -3264,28 +3288,25 @@
       <c r="E53" t="s">
         <v>26</v>
       </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
       <c r="G53" t="s">
         <v>29</v>
       </c>
       <c r="I53" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="J53" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>353</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
-        <v>357</v>
+        <v>169</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="D54" t="s">
         <v>160</v>
@@ -3293,22 +3314,19 @@
       <c r="E54" t="s">
         <v>26</v>
       </c>
-      <c r="F54" t="s">
-        <v>26</v>
-      </c>
       <c r="I54" t="s">
-        <v>358</v>
+        <v>170</v>
       </c>
       <c r="J54" t="s">
-        <v>359</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>360</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
-        <v>361</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
@@ -3322,25 +3340,28 @@
       <c r="F55" t="s">
         <v>26</v>
       </c>
+      <c r="G55" t="s">
+        <v>29</v>
+      </c>
       <c r="I55" t="s">
-        <v>362</v>
+        <v>174</v>
       </c>
       <c r="J55" t="s">
-        <v>363</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>353</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>357</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E56" t="s">
         <v>26</v>
@@ -3349,21 +3370,24 @@
         <v>26</v>
       </c>
       <c r="I56" t="s">
-        <v>179</v>
+        <v>358</v>
+      </c>
+      <c r="J56" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>176</v>
+        <v>360</v>
       </c>
       <c r="B57" t="s">
-        <v>180</v>
+        <v>361</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E57" t="s">
         <v>26</v>
@@ -3372,61 +3396,64 @@
         <v>26</v>
       </c>
       <c r="I57" t="s">
-        <v>181</v>
+        <v>362</v>
+      </c>
+      <c r="J57" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>347</v>
+        <v>178</v>
       </c>
       <c r="E58" t="s">
         <v>26</v>
       </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
       <c r="I58" t="s">
-        <v>183</v>
-      </c>
-      <c r="J58" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>348</v>
+        <v>178</v>
       </c>
       <c r="E59" t="s">
         <v>26</v>
       </c>
+      <c r="F59" t="s">
+        <v>26</v>
+      </c>
       <c r="I59" t="s">
-        <v>183</v>
-      </c>
-      <c r="J59" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>334</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C60" t="s">
         <v>25</v>
@@ -3437,25 +3464,19 @@
       <c r="E60" t="s">
         <v>26</v>
       </c>
-      <c r="F60" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" t="s">
-        <v>346</v>
-      </c>
       <c r="I60" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J60" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>334</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C61" t="s">
         <v>25</v>
@@ -3466,22 +3487,16 @@
       <c r="E61" t="s">
         <v>26</v>
       </c>
-      <c r="F61" t="s">
-        <v>26</v>
-      </c>
-      <c r="G61" t="s">
-        <v>346</v>
-      </c>
       <c r="I61" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J61" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B62" t="s">
         <v>185</v>
@@ -3510,7 +3525,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B63" t="s">
         <v>185</v>
@@ -3539,16 +3554,16 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="E64" t="s">
         <v>26</v>
@@ -3556,94 +3571,103 @@
       <c r="F64" t="s">
         <v>26</v>
       </c>
+      <c r="G64" t="s">
+        <v>346</v>
+      </c>
       <c r="I64" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J64" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="B65" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C65" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>190</v>
+        <v>348</v>
       </c>
       <c r="E65" t="s">
         <v>26</v>
       </c>
+      <c r="F65" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" t="s">
+        <v>346</v>
+      </c>
       <c r="I65" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="J65" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E66" t="s">
         <v>26</v>
       </c>
+      <c r="F66" t="s">
+        <v>26</v>
+      </c>
       <c r="I66" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="J66" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>324</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E67" t="s">
         <v>26</v>
       </c>
-      <c r="G67" t="s">
-        <v>29</v>
-      </c>
       <c r="I67" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="J67" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="D68" t="s">
         <v>199</v>
@@ -3651,250 +3675,238 @@
       <c r="E68" t="s">
         <v>26</v>
       </c>
-      <c r="G68" t="s">
-        <v>29</v>
-      </c>
       <c r="I68" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J68" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>324</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>25</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E69" t="s">
         <v>26</v>
       </c>
+      <c r="G69" t="s">
+        <v>29</v>
+      </c>
       <c r="I69" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J69" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="E70" t="s">
         <v>26</v>
       </c>
-      <c r="F70" t="s">
-        <v>26</v>
+      <c r="G70" t="s">
+        <v>29</v>
       </c>
       <c r="I70" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="J70" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>326</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="D71" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="E71" t="s">
         <v>26</v>
       </c>
-      <c r="F71" t="s">
-        <v>26</v>
-      </c>
       <c r="I71" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J71" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B72" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
-        <v>121</v>
+        <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="E72" t="s">
         <v>26</v>
       </c>
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
       <c r="I72" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="J72" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>326</v>
       </c>
       <c r="B73" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>228</v>
+        <v>75</v>
+      </c>
+      <c r="E73" t="s">
+        <v>26</v>
       </c>
       <c r="F73" t="s">
         <v>26</v>
       </c>
       <c r="I73" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="J73" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="B74" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="D74" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E74" t="s">
         <v>26</v>
       </c>
       <c r="I74" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J74" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>336</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C75" t="s">
-        <v>165</v>
+        <v>22</v>
       </c>
       <c r="D75" t="s">
-        <v>93</v>
-      </c>
-      <c r="E75" t="s">
+        <v>228</v>
+      </c>
+      <c r="F75" t="s">
         <v>26</v>
       </c>
       <c r="I75" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J75" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>234</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E76" t="s">
         <v>26</v>
       </c>
-      <c r="F76" t="s">
-        <v>26</v>
-      </c>
-      <c r="G76" t="s">
-        <v>236</v>
-      </c>
-      <c r="H76">
-        <v>300</v>
-      </c>
       <c r="I76" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="J76" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>336</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E77" t="s">
         <v>26</v>
       </c>
-      <c r="F77" t="s">
-        <v>26</v>
-      </c>
-      <c r="G77" t="s">
-        <v>29</v>
-      </c>
-      <c r="H77">
-        <v>20</v>
-      </c>
       <c r="I77" t="s">
-        <v>241</v>
+        <v>232</v>
+      </c>
+      <c r="J77" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="B78" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C78" t="s">
         <v>25</v>
@@ -3909,24 +3921,27 @@
         <v>26</v>
       </c>
       <c r="G78" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H78">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="I78" t="s">
-        <v>244</v>
+        <v>237</v>
+      </c>
+      <c r="J78" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B79" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -3934,25 +3949,28 @@
       <c r="E79" t="s">
         <v>26</v>
       </c>
+      <c r="F79" t="s">
+        <v>26</v>
+      </c>
       <c r="G79" t="s">
         <v>29</v>
       </c>
+      <c r="H79">
+        <v>20</v>
+      </c>
       <c r="I79" t="s">
-        <v>247</v>
-      </c>
-      <c r="J79" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C80" t="s">
-        <v>341</v>
+        <v>25</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
@@ -3960,14 +3978,17 @@
       <c r="E80" t="s">
         <v>26</v>
       </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
       <c r="G80" t="s">
-        <v>29</v>
+        <v>243</v>
+      </c>
+      <c r="H80">
+        <v>50</v>
       </c>
       <c r="I80" t="s">
-        <v>247</v>
-      </c>
-      <c r="J80" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -3975,10 +3996,10 @@
         <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
@@ -3989,25 +4010,22 @@
       <c r="G81" t="s">
         <v>29</v>
       </c>
-      <c r="H81">
-        <v>2</v>
-      </c>
       <c r="I81" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="J81" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B82" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C82" t="s">
-        <v>25</v>
+        <v>341</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -4015,94 +4033,149 @@
       <c r="E82" t="s">
         <v>26</v>
       </c>
-      <c r="F82" t="s">
-        <v>26</v>
-      </c>
-      <c r="H82" t="s">
-        <v>254</v>
+      <c r="G82" t="s">
+        <v>29</v>
       </c>
       <c r="I82" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J82" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C83" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="G83" t="s">
+        <v>29</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
       </c>
       <c r="I83" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="J83" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B84" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
-        <v>341</v>
+        <v>25</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F84" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="H84" t="s">
+        <v>254</v>
       </c>
       <c r="I84" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J84" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>315</v>
+        <v>257</v>
       </c>
       <c r="B85" t="s">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="C85" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F85" t="s">
         <v>155</v>
       </c>
       <c r="I85" t="s">
+        <v>259</v>
+      </c>
+      <c r="J85" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>257</v>
+      </c>
+      <c r="B86" t="s">
+        <v>258</v>
+      </c>
+      <c r="C86" t="s">
+        <v>341</v>
+      </c>
+      <c r="D86" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" t="s">
+        <v>155</v>
+      </c>
+      <c r="I86" t="s">
+        <v>259</v>
+      </c>
+      <c r="J86" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>315</v>
+      </c>
+      <c r="B87" t="s">
+        <v>316</v>
+      </c>
+      <c r="C87" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" t="s">
+        <v>155</v>
+      </c>
+      <c r="I87" t="s">
         <v>317</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J87" t="s">
         <v>318</v>
       </c>
     </row>

</xml_diff>